<commit_message>
making tests and changing combinations
</commit_message>
<xml_diff>
--- a/Investimento_x_Venda.xlsx
+++ b/Investimento_x_Venda.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26424"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conta\Documents\#\Regressao ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E035B461-BD1C-46A3-A7A2-03A04E26D13C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5088AA3C-E380-43FF-8768-41320A4F938F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C0D891DA-7B4E-4336-9BCC-6E42B911F749}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,7 @@
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -47,8 +48,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -76,9 +85,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -234,10 +246,10 @@
                   <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>72</c:v>
+                  <c:v>75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>81</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -264,10 +276,10 @@
                   <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>335</c:v>
+                  <c:v>342</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>364</c:v>
+                  <c:v>387</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1064,7 +1076,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1360,19 +1372,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC214589-2CE2-4C73-8191-98F685E23ED4}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R12" sqref="R12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="29.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="22.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1392,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1">
         <v>20</v>
       </c>
@@ -1388,7 +1400,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1">
         <v>25</v>
       </c>
@@ -1396,7 +1408,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1">
         <v>40</v>
       </c>
@@ -1404,7 +1416,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1">
         <v>52</v>
       </c>
@@ -1412,7 +1424,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1">
         <v>67</v>
       </c>
@@ -1420,21 +1432,27 @@
         <v>295</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B7" s="1">
-        <v>335</v>
+        <v>342</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="1">
-        <v>364</v>
-      </c>
+        <v>387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="2"/>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
adicionando ROI e corrigindo database
</commit_message>
<xml_diff>
--- a/Investimento_x_Venda.xlsx
+++ b/Investimento_x_Venda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conta\Documents\#\Regressao ML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5088AA3C-E380-43FF-8768-41320A4F938F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FEFBA7A-5214-4C54-9928-F39D15C713B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{C0D891DA-7B4E-4336-9BCC-6E42B911F749}"/>
   </bookViews>
@@ -246,10 +246,10 @@
                   <c:v>67</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>75</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -273,13 +273,13 @@
                   <c:v>260</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>295</c:v>
+                  <c:v>320</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>342</c:v>
+                  <c:v>335</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>387</c:v>
+                  <c:v>364</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1375,7 +1375,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1429,23 +1429,23 @@
         <v>67</v>
       </c>
       <c r="B6" s="1">
-        <v>295</v>
+        <v>320</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B7" s="1">
-        <v>342</v>
+        <v>335</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B8" s="1">
-        <v>387</v>
+        <v>364</v>
       </c>
     </row>
     <row r="11" spans="1:2">

</xml_diff>